<commit_message>
Added Dell Command | Update
Signed-off-by: Josue Negron <jnegron@vmware.com>
</commit_message>
<xml_diff>
--- a/Windows-Samples/Tools & Utilities/Software Distribution Templates/Validated App Templates.xlsx
+++ b/Windows-Samples/Tools & Utilities/Software Distribution Templates/Validated App Templates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnegron\OneDrive - VMware, Inc\EUC Tech Marketing\Code\Git\Windows-Samples\Tools &amp; Utilities\Software Distribution Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="17" documentId="7C7ACA746296BA24F4C321B768968F40ED574D1F" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{1103C65A-78EF-460B-B6E0-C5E92FD5DFDA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apps" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="228">
   <si>
     <t>Details</t>
   </si>
@@ -773,11 +774,38 @@
   <si>
     <t>Teams_windows_x64.exe /s</t>
   </si>
+  <si>
+    <t>Dell Command | Update</t>
+  </si>
+  <si>
+    <t>2.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://downloads.dell.com/FOLDER04358530M/1/Dell-Command-Update_X79N4_WIN_2.3.1_A00.EXE </t>
+  </si>
+  <si>
+    <t>Dell-Command-Update_X79N4_WIN_2.3.1_A00.EXE</t>
+  </si>
+  <si>
+    <t>msiexec /x {EC542D5D-B608-4145-A8F7-749C02BE6D94} /qn</t>
+  </si>
+  <si>
+    <t>Dell-Command-Update_X79N4_WIN_2.3.1_A00.EXE /s</t>
+  </si>
+  <si>
+    <t>Key: HKLM\SOFTWARE\WOW6432Node\Microsoft\Windows\CurrentVersion\Uninstall\{EC542D5D-B608-4145-A8F7-749C02BE6D94}
+SubKey: DisplayName
+Type: String
+Value: Dell Command | Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://i.imgur.com/NzeHcWP.png </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1064,33 +1092,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:U34" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A2:U34"/>
-  <sortState ref="A3:U34">
-    <sortCondition ref="A2:A34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:U35" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A2:U35" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState ref="A3:U35">
+    <sortCondition ref="A2:A35"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="1" name="Name" dataDxfId="20"/>
-    <tableColumn id="2" name="Version" dataDxfId="19"/>
-    <tableColumn id="3" name="Architecture" dataDxfId="18"/>
-    <tableColumn id="21" name="Download Package" dataDxfId="17"/>
-    <tableColumn id="19" name="File Name" dataDxfId="16"/>
-    <tableColumn id="4" name="App Dependencies" dataDxfId="15"/>
-    <tableColumn id="5" name="App Uninstall Process" dataDxfId="14"/>
-    <tableColumn id="6" name="Disk Space" dataDxfId="13"/>
-    <tableColumn id="7" name="Device Power" dataDxfId="12"/>
-    <tableColumn id="8" name="RAM" dataDxfId="11"/>
-    <tableColumn id="9" name="Install Context" dataDxfId="10"/>
-    <tableColumn id="10" name="Install Command" dataDxfId="9"/>
-    <tableColumn id="11" name="Admin Privileges" dataDxfId="8"/>
-    <tableColumn id="12" name="Retry Count" dataDxfId="7"/>
-    <tableColumn id="13" name="Retry Interval" dataDxfId="6"/>
-    <tableColumn id="14" name="Install Timeout" dataDxfId="5"/>
-    <tableColumn id="15" name="Reboot Exit Code" dataDxfId="4"/>
-    <tableColumn id="16" name="Success Exit Code" dataDxfId="3"/>
-    <tableColumn id="17" name="When To Call Install Complete" dataDxfId="2"/>
-    <tableColumn id="18" name="Icon" dataDxfId="1"/>
-    <tableColumn id="20" name="Notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Version" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Architecture" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Download Package" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="File Name" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="App Dependencies" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="App Uninstall Process" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Disk Space" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Device Power" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="RAM" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Install Context" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Install Command" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Admin Privileges" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Retry Count" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Retry Interval" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Install Timeout" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Reboot Exit Code" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Success Exit Code" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="When To Call Install Complete" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1392,12 +1420,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1816,40 +1844,34 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="57" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>78</v>
+        <v>220</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>79</v>
+        <v>221</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>80</v>
+        <v>222</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>81</v>
+        <v>223</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>82</v>
+        <v>224</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="K12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>84</v>
+        <v>225</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>42</v>
@@ -1857,758 +1879,806 @@
       <c r="P12" s="1">
         <v>20</v>
       </c>
-      <c r="Q12" s="1">
-        <v>1614</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0</v>
-      </c>
       <c r="S12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
+        <v>226</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="57" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>89</v>
+      <c r="D13" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N13" s="1">
-        <v>3</v>
-      </c>
-      <c r="O13" s="1">
-        <v>5</v>
-      </c>
       <c r="P13" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q13" s="1">
-        <v>1</v>
+        <v>1614</v>
       </c>
       <c r="R13" s="1">
         <v>0</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="4">
-        <v>54</v>
+      <c r="B14" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="E14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="1">
+        <v>3</v>
+      </c>
+      <c r="O14" s="1">
+        <v>5</v>
+      </c>
+      <c r="P14" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="4">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="L14" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="T14" s="7"/>
-    </row>
-    <row r="15" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="F15" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="I15" s="3"/>
       <c r="L15" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>105</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="T15" s="7"/>
     </row>
     <row r="16" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="I16" s="3"/>
       <c r="L16" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R16" s="1">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>30</v>
+        <v>110</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="K17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="L17" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17" s="1">
-        <v>30</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>1614</v>
+        <v>29</v>
       </c>
       <c r="R17" s="1">
         <v>0</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="T17" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="U17" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="K18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="1">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>1614</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>126</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="L18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S18" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="114" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="I19" s="3"/>
       <c r="L19" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="114" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>136</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="I20" s="3"/>
       <c r="L20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="L21" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="S20" s="4" t="s">
+      <c r="S21" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A21" s="4" t="s">
+    <row r="22" spans="1:21" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="F22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
         <v>144</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="K21" s="1" t="s">
+      <c r="I22" s="3"/>
+      <c r="K22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q21" s="1">
+      <c r="M22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="1">
         <v>1614</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R22" s="1">
         <v>0</v>
       </c>
-      <c r="S21" s="4" t="s">
+      <c r="S22" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="114" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="F23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="L22" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>155</v>
       </c>
       <c r="I23" s="3"/>
       <c r="L23" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>42</v>
+        <v>151</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>160</v>
-      </c>
       <c r="E24" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>162</v>
+        <v>154</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>155</v>
       </c>
       <c r="I24" s="3"/>
       <c r="L24" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R24" s="1">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="L25" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="4" t="s">
+      <c r="F26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="K25" s="1" t="s">
+      <c r="I26" s="3"/>
+      <c r="K26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L26" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N25" s="1">
+      <c r="M26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N26" s="1">
         <v>0</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O26" s="1">
         <v>5</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P26" s="1">
         <v>20</v>
       </c>
-      <c r="Q25" s="1">
+      <c r="Q26" s="1">
         <v>1614</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="S26" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:21" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:21" ht="57" x14ac:dyDescent="0.45">
-      <c r="A27" s="4" t="s">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:21" ht="57" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B28" s="4">
         <v>2.7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="I27" s="3"/>
-      <c r="K27" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N27" s="1">
-        <v>1</v>
-      </c>
-      <c r="O27" s="1">
-        <v>5</v>
-      </c>
-      <c r="P27" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q27" s="1">
-        <v>3010</v>
-      </c>
-      <c r="R27" s="1">
-        <v>0</v>
-      </c>
-      <c r="S27" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="T27" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="U27" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="114" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>177</v>
+      </c>
       <c r="E28" s="4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="G28" s="4" t="s">
+        <v>179</v>
+      </c>
       <c r="I28" s="3"/>
+      <c r="K28" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="L28" s="4" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="N28" s="1">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>5</v>
+      </c>
+      <c r="P28" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>3010</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="T28" s="5"/>
-      <c r="U28" s="11"/>
+        <v>181</v>
+      </c>
+      <c r="T28" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="U28" s="11" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="29" spans="1:21" ht="114" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="I29" s="3"/>
       <c r="L29" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="T29" s="5"/>
       <c r="U29" s="11"/>
     </row>
-    <row r="30" spans="1:21" ht="57" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:21" ht="114" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>214</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="4" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>216</v>
-      </c>
       <c r="I30" s="3"/>
-      <c r="K30" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="L30" s="4" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+      <c r="T30" s="5"/>
+      <c r="U30" s="11"/>
+    </row>
+    <row r="31" spans="1:21" ht="57" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="4" t="s">
+        <v>214</v>
+      </c>
       <c r="E31" s="4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>194</v>
+        <v>29</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>216</v>
       </c>
       <c r="I31" s="3"/>
+      <c r="K31" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="L31" s="4" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="T31" s="5"/>
-      <c r="U31" s="11" t="s">
-        <v>197</v>
+        <v>218</v>
+      </c>
+      <c r="T31" s="4" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="114" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="I32" s="3"/>
       <c r="L32" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="T32" s="5"/>
+      <c r="U32" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+      <c r="A33" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S32" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="T32" s="5"/>
-      <c r="U32" s="11"/>
-    </row>
-    <row r="33" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F33" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="K33" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="L33" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="S33" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="T33" s="5"/>
+      <c r="U33" s="11"/>
+    </row>
+    <row r="34" spans="1:21" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="K34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S34" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="114" x14ac:dyDescent="0.45">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:21" ht="114" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="L34" s="4" t="s">
+      <c r="I35" s="3"/>
+      <c r="L35" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S34" s="4" t="s">
+      <c r="M35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S35" s="4" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2619,30 +2689,33 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D16" r:id="rId1"/>
-    <hyperlink ref="D15" r:id="rId2"/>
-    <hyperlink ref="D24" r:id="rId3"/>
-    <hyperlink ref="D7" r:id="rId4"/>
-    <hyperlink ref="D25" r:id="rId5"/>
-    <hyperlink ref="D9" r:id="rId6"/>
-    <hyperlink ref="D18" r:id="rId7"/>
-    <hyperlink ref="D20" r:id="rId8"/>
-    <hyperlink ref="T10" r:id="rId9"/>
-    <hyperlink ref="T27" r:id="rId10"/>
-    <hyperlink ref="D26" r:id="rId11"/>
-    <hyperlink ref="D17" r:id="rId12"/>
-    <hyperlink ref="D3" r:id="rId13"/>
-    <hyperlink ref="D4" r:id="rId14"/>
-    <hyperlink ref="D27" r:id="rId15"/>
-    <hyperlink ref="D12" r:id="rId16"/>
-    <hyperlink ref="D13" r:id="rId17"/>
-    <hyperlink ref="T13" r:id="rId18"/>
-    <hyperlink ref="D8" r:id="rId19"/>
+    <hyperlink ref="D17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D25" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D26" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D19" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D21" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="T10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="T28" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D3" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D4" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D28" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D13" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D14" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="T14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D12" r:id="rId20" xr:uid="{0CC64C78-B4AA-4A7A-B130-26DA462B898A}"/>
+    <hyperlink ref="T13" r:id="rId21" xr:uid="{57B690FD-2F50-4D6C-A63B-67E06691524E}"/>
+    <hyperlink ref="T12" r:id="rId22" xr:uid="{776BA159-34A9-4023-BCA9-9C0FC44744FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
   <tableParts count="1">
-    <tablePart r:id="rId21"/>
+    <tablePart r:id="rId24"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>